<commit_message>
added classes for data
</commit_message>
<xml_diff>
--- a/Witchborn Database.xlsx
+++ b/Witchborn Database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dJoeC\Witchborn-Roster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D630F880-AD8D-438A-93B4-93818920F09A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{674B261E-8208-4287-AF12-6C945EBC284C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12480" yWindow="3465" windowWidth="13470" windowHeight="15435" activeTab="3" xr2:uid="{BD116EAC-F748-44A7-BC83-C22CD1D19B13}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="18220" windowHeight="11620" activeTab="3" xr2:uid="{BD116EAC-F748-44A7-BC83-C22CD1D19B13}"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
@@ -2441,14 +2441,14 @@
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="1"/>
-    <col min="14" max="14" width="44.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" style="1"/>
+    <col min="14" max="14" width="44.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2492,7 +2492,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2550,7 +2550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -2608,7 +2608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -2637,7 +2637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -2666,7 +2666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -2695,7 +2695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -2727,7 +2727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -2756,7 +2756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -2788,7 +2788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -2817,7 +2817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -2846,7 +2846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -2904,7 +2904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -2936,7 +2936,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -3000,7 +3000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -3032,7 +3032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -3064,7 +3064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -3102,7 +3102,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -3137,7 +3137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -3175,7 +3175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>148</v>
       </c>
@@ -3204,7 +3204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>148</v>
       </c>
@@ -3233,7 +3233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>148</v>
       </c>
@@ -3262,7 +3262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>148</v>
       </c>
@@ -3294,7 +3294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>148</v>
       </c>
@@ -3323,7 +3323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>148</v>
       </c>
@@ -3352,7 +3352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>148</v>
       </c>
@@ -3381,7 +3381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>148</v>
       </c>
@@ -3413,7 +3413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>148</v>
       </c>
@@ -3445,7 +3445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>148</v>
       </c>
@@ -3474,7 +3474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>148</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>148</v>
       </c>
@@ -3535,7 +3535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>148</v>
       </c>
@@ -3570,7 +3570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>148</v>
       </c>
@@ -3602,7 +3602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>148</v>
       </c>
@@ -3634,7 +3634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>148</v>
       </c>
@@ -3660,7 +3660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>148</v>
       </c>
@@ -3705,19 +3705,19 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:A19"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="21.28515625" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="93.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.26953125" customWidth="1"/>
+    <col min="3" max="3" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.1796875" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="93.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3746,7 +3746,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -3769,7 +3769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -3792,7 +3792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -3818,7 +3818,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -3841,7 +3841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -3867,7 +3867,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -3893,7 +3893,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -3916,7 +3916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -3939,7 +3939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>148</v>
       </c>
@@ -3962,7 +3962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>148</v>
       </c>
@@ -3985,7 +3985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>148</v>
       </c>
@@ -4008,7 +4008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>148</v>
       </c>
@@ -4034,7 +4034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>148</v>
       </c>
@@ -4057,7 +4057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>148</v>
       </c>
@@ -4083,7 +4083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>148</v>
       </c>
@@ -4112,7 +4112,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>148</v>
       </c>
@@ -4135,7 +4135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>148</v>
       </c>
@@ -4161,7 +4161,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>148</v>
       </c>
@@ -4200,13 +4200,13 @@
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4229,7 +4229,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -4249,7 +4249,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -4269,7 +4269,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -4289,7 +4289,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -4309,7 +4309,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -4329,7 +4329,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -4349,7 +4349,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -4369,7 +4369,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -4389,7 +4389,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -4409,7 +4409,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -4429,7 +4429,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -4449,7 +4449,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -4469,7 +4469,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -4489,7 +4489,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -4509,7 +4509,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -4529,7 +4529,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -4549,7 +4549,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -4572,7 +4572,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -4592,7 +4592,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -4615,7 +4615,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -4635,7 +4635,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -4655,7 +4655,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -4678,7 +4678,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -4698,7 +4698,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -4721,7 +4721,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -4741,7 +4741,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -4761,7 +4761,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -4781,7 +4781,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -4801,7 +4801,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -4821,7 +4821,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>1</v>
       </c>
@@ -4841,7 +4841,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>1</v>
       </c>
@@ -4861,7 +4861,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>1</v>
       </c>
@@ -4881,7 +4881,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>1</v>
       </c>
@@ -4901,7 +4901,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>1</v>
       </c>
@@ -4921,7 +4921,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>1</v>
       </c>
@@ -4944,7 +4944,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>1</v>
       </c>
@@ -4964,7 +4964,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>1</v>
       </c>
@@ -4984,7 +4984,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>1</v>
       </c>
@@ -5004,7 +5004,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>1</v>
       </c>
@@ -5024,7 +5024,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>1</v>
       </c>
@@ -5044,7 +5044,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>1</v>
       </c>
@@ -5064,7 +5064,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>1</v>
       </c>
@@ -5084,7 +5084,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>1</v>
       </c>
@@ -5104,7 +5104,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>1</v>
       </c>
@@ -5121,7 +5121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>148</v>
       </c>
@@ -5144,7 +5144,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>148</v>
       </c>
@@ -5164,7 +5164,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>148</v>
       </c>
@@ -5184,7 +5184,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>148</v>
       </c>
@@ -5204,7 +5204,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>148</v>
       </c>
@@ -5224,7 +5224,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>148</v>
       </c>
@@ -5247,7 +5247,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>148</v>
       </c>
@@ -5267,7 +5267,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>148</v>
       </c>
@@ -5287,7 +5287,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>148</v>
       </c>
@@ -5307,7 +5307,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>148</v>
       </c>
@@ -5327,7 +5327,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>148</v>
       </c>
@@ -5347,7 +5347,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>148</v>
       </c>
@@ -5367,7 +5367,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>148</v>
       </c>
@@ -5387,7 +5387,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>148</v>
       </c>
@@ -5410,7 +5410,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>148</v>
       </c>
@@ -5430,7 +5430,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>148</v>
       </c>
@@ -5453,7 +5453,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>148</v>
       </c>
@@ -5473,7 +5473,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>148</v>
       </c>
@@ -5493,7 +5493,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>148</v>
       </c>
@@ -5513,7 +5513,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>148</v>
       </c>
@@ -5533,7 +5533,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>148</v>
       </c>
@@ -5553,7 +5553,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>148</v>
       </c>
@@ -5573,7 +5573,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>148</v>
       </c>
@@ -5593,7 +5593,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>148</v>
       </c>
@@ -5613,7 +5613,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>148</v>
       </c>
@@ -5636,7 +5636,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>148</v>
       </c>
@@ -5656,7 +5656,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>148</v>
       </c>
@@ -5676,7 +5676,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>148</v>
       </c>
@@ -5696,7 +5696,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>148</v>
       </c>
@@ -5719,7 +5719,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>148</v>
       </c>
@@ -5739,7 +5739,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>148</v>
       </c>
@@ -5759,7 +5759,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>148</v>
       </c>
@@ -5779,7 +5779,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>148</v>
       </c>
@@ -5799,7 +5799,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>148</v>
       </c>
@@ -5828,20 +5828,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{928C73B0-E9CF-4897-9791-F504AFAA1ADB}">
   <dimension ref="A1:F172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="F176" sqref="F176"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" customWidth="1"/>
-    <col min="6" max="6" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7265625" customWidth="1"/>
+    <col min="4" max="4" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.81640625" customWidth="1"/>
+    <col min="6" max="6" width="255.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>355</v>
       </c>
@@ -5861,7 +5861,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -5878,7 +5878,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -5895,7 +5895,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -5912,7 +5912,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -5929,7 +5929,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -5943,7 +5943,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -5960,7 +5960,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -5977,7 +5977,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -5994,7 +5994,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -6008,7 +6008,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -6022,7 +6022,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -6039,7 +6039,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -6053,7 +6053,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -6070,7 +6070,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -6090,7 +6090,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -6107,7 +6107,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -6124,7 +6124,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -6141,7 +6141,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>148</v>
       </c>
@@ -6161,7 +6161,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>148</v>
       </c>
@@ -6175,7 +6175,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>148</v>
       </c>
@@ -6192,7 +6192,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>148</v>
       </c>
@@ -6212,7 +6212,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>148</v>
       </c>
@@ -6229,7 +6229,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>148</v>
       </c>
@@ -6246,7 +6246,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>148</v>
       </c>
@@ -6263,7 +6263,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>148</v>
       </c>
@@ -6283,7 +6283,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>148</v>
       </c>
@@ -6300,7 +6300,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>148</v>
       </c>
@@ -6314,7 +6314,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>148</v>
       </c>
@@ -6331,7 +6331,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>148</v>
       </c>
@@ -6348,7 +6348,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>148</v>
       </c>
@@ -6368,7 +6368,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>148</v>
       </c>
@@ -6385,7 +6385,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>148</v>
       </c>
@@ -6402,7 +6402,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>148</v>
       </c>
@@ -6419,7 +6419,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>341</v>
       </c>
@@ -6436,7 +6436,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>341</v>
       </c>
@@ -6450,7 +6450,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>341</v>
       </c>
@@ -6467,7 +6467,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>330</v>
       </c>
@@ -6481,7 +6481,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>333</v>
       </c>
@@ -6501,7 +6501,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>330</v>
       </c>
@@ -6521,7 +6521,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>341</v>
       </c>
@@ -6535,7 +6535,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>341</v>
       </c>
@@ -6549,7 +6549,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>341</v>
       </c>
@@ -6563,7 +6563,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>330</v>
       </c>
@@ -6580,7 +6580,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>351</v>
       </c>
@@ -6597,7 +6597,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>351</v>
       </c>
@@ -6617,7 +6617,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>341</v>
       </c>
@@ -6634,7 +6634,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>361</v>
       </c>
@@ -6651,7 +6651,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>333</v>
       </c>
@@ -6668,7 +6668,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>341</v>
       </c>
@@ -6685,7 +6685,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>333</v>
       </c>
@@ -6702,7 +6702,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>351</v>
       </c>
@@ -6716,7 +6716,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>333</v>
       </c>
@@ -6730,7 +6730,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>36</v>
       </c>
@@ -6750,7 +6750,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>361</v>
       </c>
@@ -6767,7 +6767,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>333</v>
       </c>
@@ -6787,7 +6787,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>341</v>
       </c>
@@ -6804,7 +6804,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>36</v>
       </c>
@@ -6821,7 +6821,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>341</v>
       </c>
@@ -6835,7 +6835,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>341</v>
       </c>
@@ -6849,7 +6849,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>341</v>
       </c>
@@ -6863,7 +6863,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>361</v>
       </c>
@@ -6880,7 +6880,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>341</v>
       </c>
@@ -6894,7 +6894,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>351</v>
       </c>
@@ -6911,7 +6911,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>333</v>
       </c>
@@ -6928,7 +6928,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>330</v>
       </c>
@@ -6945,7 +6945,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>341</v>
       </c>
@@ -6959,7 +6959,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>36</v>
       </c>
@@ -6973,7 +6973,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>36</v>
       </c>
@@ -6990,7 +6990,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>330</v>
       </c>
@@ -7010,7 +7010,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>36</v>
       </c>
@@ -7027,7 +7027,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>351</v>
       </c>
@@ -7047,7 +7047,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>341</v>
       </c>
@@ -7061,7 +7061,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>361</v>
       </c>
@@ -7075,7 +7075,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>330</v>
       </c>
@@ -7092,7 +7092,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>330</v>
       </c>
@@ -7112,7 +7112,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>36</v>
       </c>
@@ -7129,7 +7129,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>361</v>
       </c>
@@ -7146,7 +7146,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>361</v>
       </c>
@@ -7163,7 +7163,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>341</v>
       </c>
@@ -7177,7 +7177,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>341</v>
       </c>
@@ -7191,7 +7191,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>341</v>
       </c>
@@ -7208,7 +7208,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>341</v>
       </c>
@@ -7222,7 +7222,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>341</v>
       </c>
@@ -7236,7 +7236,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>330</v>
       </c>
@@ -7253,7 +7253,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>361</v>
       </c>
@@ -7270,7 +7270,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>330</v>
       </c>
@@ -7287,7 +7287,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>341</v>
       </c>
@@ -7304,7 +7304,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>351</v>
       </c>
@@ -7318,7 +7318,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>341</v>
       </c>
@@ -7332,7 +7332,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>341</v>
       </c>
@@ -7346,7 +7346,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>333</v>
       </c>
@@ -7357,7 +7357,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>333</v>
       </c>
@@ -7377,7 +7377,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>341</v>
       </c>
@@ -7391,7 +7391,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>333</v>
       </c>
@@ -7411,7 +7411,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>330</v>
       </c>
@@ -7425,7 +7425,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>341</v>
       </c>
@@ -7439,7 +7439,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>330</v>
       </c>
@@ -7456,7 +7456,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>341</v>
       </c>
@@ -7470,7 +7470,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>341</v>
       </c>
@@ -7484,7 +7484,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>341</v>
       </c>
@@ -7498,7 +7498,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>333</v>
       </c>
@@ -7518,7 +7518,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>341</v>
       </c>
@@ -7532,7 +7532,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>341</v>
       </c>
@@ -7549,7 +7549,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>341</v>
       </c>
@@ -7563,7 +7563,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>36</v>
       </c>
@@ -7577,7 +7577,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>361</v>
       </c>
@@ -7597,7 +7597,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>361</v>
       </c>
@@ -7614,7 +7614,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>341</v>
       </c>
@@ -7628,7 +7628,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>341</v>
       </c>
@@ -7645,7 +7645,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>341</v>
       </c>
@@ -7662,7 +7662,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>361</v>
       </c>
@@ -7676,7 +7676,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>333</v>
       </c>
@@ -7693,7 +7693,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>341</v>
       </c>
@@ -7707,7 +7707,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>341</v>
       </c>
@@ -7724,7 +7724,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>361</v>
       </c>
@@ -7738,7 +7738,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>341</v>
       </c>
@@ -7752,7 +7752,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>333</v>
       </c>
@@ -7772,7 +7772,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>361</v>
       </c>
@@ -7789,7 +7789,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>341</v>
       </c>
@@ -7803,7 +7803,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>351</v>
       </c>
@@ -7823,7 +7823,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>341</v>
       </c>
@@ -7837,7 +7837,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>341</v>
       </c>
@@ -7851,7 +7851,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>351</v>
       </c>
@@ -7871,7 +7871,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>351</v>
       </c>
@@ -7885,7 +7885,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>351</v>
       </c>
@@ -7899,7 +7899,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>330</v>
       </c>
@@ -7919,7 +7919,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>341</v>
       </c>
@@ -7936,7 +7936,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>341</v>
       </c>
@@ -7950,7 +7950,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>341</v>
       </c>
@@ -7967,7 +7967,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>36</v>
       </c>
@@ -7981,7 +7981,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>341</v>
       </c>
@@ -7998,7 +7998,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>36</v>
       </c>
@@ -8012,7 +8012,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>330</v>
       </c>
@@ -8026,7 +8026,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>341</v>
       </c>
@@ -8040,7 +8040,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>330</v>
       </c>
@@ -8057,7 +8057,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>36</v>
       </c>
@@ -8074,7 +8074,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>341</v>
       </c>
@@ -8088,7 +8088,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>361</v>
       </c>
@@ -8105,7 +8105,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>36</v>
       </c>
@@ -8125,7 +8125,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>333</v>
       </c>
@@ -8145,7 +8145,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>36</v>
       </c>
@@ -8165,7 +8165,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>351</v>
       </c>
@@ -8182,7 +8182,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>330</v>
       </c>
@@ -8199,7 +8199,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>361</v>
       </c>
@@ -8213,7 +8213,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>341</v>
       </c>
@@ -8227,7 +8227,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>330</v>
       </c>
@@ -8244,7 +8244,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>351</v>
       </c>
@@ -8261,7 +8261,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>341</v>
       </c>
@@ -8278,7 +8278,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>341</v>
       </c>
@@ -8292,7 +8292,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>361</v>
       </c>
@@ -8306,7 +8306,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>330</v>
       </c>
@@ -8320,7 +8320,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>351</v>
       </c>
@@ -8337,7 +8337,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>341</v>
       </c>
@@ -8354,7 +8354,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>341</v>
       </c>
@@ -8368,7 +8368,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>333</v>
       </c>
@@ -8385,7 +8385,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>361</v>
       </c>
@@ -8405,7 +8405,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>341</v>
       </c>
@@ -8422,7 +8422,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>341</v>
       </c>
@@ -8439,7 +8439,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>341</v>
       </c>
@@ -8453,7 +8453,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>330</v>
       </c>
@@ -8467,7 +8467,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>333</v>
       </c>
@@ -8481,7 +8481,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>333</v>
       </c>
@@ -8501,7 +8501,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>341</v>
       </c>
@@ -8515,7 +8515,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>341</v>
       </c>
@@ -8529,7 +8529,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>330</v>
       </c>
@@ -8546,7 +8546,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>341</v>
       </c>
@@ -8560,7 +8560,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>341</v>
       </c>
@@ -8574,7 +8574,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>341</v>
       </c>
@@ -8588,7 +8588,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>351</v>
       </c>
@@ -8605,7 +8605,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>341</v>
       </c>
@@ -8619,7 +8619,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>361</v>
       </c>
@@ -8638,5 +8638,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>